<commit_message>
Ajout du modèle de la bombe + MAJ historique
</commit_message>
<xml_diff>
--- a/Docs/Historique.xlsx
+++ b/Docs/Historique.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Taches</t>
   </si>
@@ -45,9 +45,6 @@
     <t>En cours</t>
   </si>
   <si>
-    <t>Construteur de map</t>
-  </si>
-  <si>
     <t>Ajout contrôle du player</t>
   </si>
   <si>
@@ -100,6 +97,15 @@
   </si>
   <si>
     <t>A faire</t>
+  </si>
+  <si>
+    <t>Constrution de la map</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Modélisation de la bombe</t>
   </si>
 </sst>
 </file>
@@ -159,15 +165,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -474,7 +480,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,391 +492,397 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Ajout texture sur bombe + Sceptre MAJ Historique.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Historique.xlsx
+++ b/Docs/Historique.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8250"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>Taches</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Modélisation player</t>
   </si>
   <si>
-    <t xml:space="preserve">Texture map + cubes + bombes + player + sceptre </t>
-  </si>
-  <si>
     <t>Sons</t>
   </si>
   <si>
@@ -115,13 +112,25 @@
   </si>
   <si>
     <t>Intégration de la bombe</t>
+  </si>
+  <si>
+    <t>Modélisation du sceptre</t>
+  </si>
+  <si>
+    <t>Texture bombes + sceptre</t>
+  </si>
+  <si>
+    <t>TP3</t>
+  </si>
+  <si>
+    <t>Texture map + cubes + player</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -386,11 +395,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,28 +472,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,6 +594,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -584,6 +629,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -759,74 +805,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="94.140625" style="24" customWidth="1"/>
     <col min="2" max="5" width="11.42578125" style="1"/>
     <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="C2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -834,39 +880,39 @@
         <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -874,19 +920,19 @@
         <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -894,7 +940,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="5"/>
@@ -902,7 +948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -910,7 +956,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5"/>
@@ -918,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -926,7 +972,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
@@ -934,7 +980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -942,7 +988,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="5"/>
@@ -950,15 +996,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
@@ -966,9 +1012,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -976,15 +1022,15 @@
         <v>14</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>14</v>
@@ -996,70 +1042,69 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -1067,7 +1112,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -1075,7 +1120,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -1083,55 +1128,71 @@
       <c r="E22" s="5"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="5"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="5"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="5"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="5"/>
+      <c r="F25" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="5"/>
+      <c r="F26" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4"/>
+      <c r="F27" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="F28" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -1139,7 +1200,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -1147,7 +1208,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -1155,7 +1216,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -1163,7 +1224,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -1171,7 +1232,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -1179,7 +1240,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1187,7 +1248,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1195,7 +1256,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1203,7 +1264,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1211,7 +1272,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1219,7 +1280,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1227,7 +1288,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1235,7 +1296,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1243,7 +1304,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1251,7 +1312,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1259,7 +1320,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1267,7 +1328,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1275,7 +1336,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1283,7 +1344,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1291,7 +1352,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1299,7 +1360,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1307,7 +1368,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1328,24 +1389,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Met à jour l'historique
</commit_message>
<xml_diff>
--- a/Docs/Historique.xlsx
+++ b/Docs/Historique.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8250"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Taches</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>Texture map + cubes + player</t>
+  </si>
+  <si>
+    <t>Chargement des niveaux depuis un fichier</t>
+  </si>
+  <si>
+    <t>1h30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,18 +490,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -503,6 +497,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -594,7 +600,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -629,7 +634,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -805,39 +809,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="94.140625" style="24" customWidth="1"/>
+    <col min="1" max="1" width="94.140625" style="20" customWidth="1"/>
     <col min="2" max="5" width="11.42578125" style="1"/>
     <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="22"/>
       <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
@@ -850,9 +854,9 @@
       <c r="E2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="23"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -872,7 +876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -892,7 +896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -912,7 +916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -932,7 +936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -948,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -964,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -980,7 +984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1012,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1056,8 +1060,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="7"/>
@@ -1072,15 +1076,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -1088,7 +1100,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -1096,7 +1108,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -1104,7 +1116,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -1112,7 +1124,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
@@ -1120,7 +1132,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
@@ -1128,7 +1140,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -1136,7 +1148,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
@@ -1144,7 +1156,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1180,7 +1192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1192,7 +1204,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="4"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
@@ -1200,7 +1212,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="4"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
@@ -1208,7 +1220,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="4"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -1216,7 +1228,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="4"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -1224,7 +1236,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="4"/>
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
@@ -1232,7 +1244,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="4"/>
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
@@ -1240,7 +1252,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1248,7 +1260,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1256,7 +1268,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1264,7 +1276,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1272,7 +1284,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1280,7 +1292,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1288,7 +1300,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1296,7 +1308,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1304,7 +1316,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1312,7 +1324,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1320,7 +1332,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1328,7 +1340,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1336,7 +1348,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1344,7 +1356,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1352,7 +1364,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1360,7 +1372,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1368,7 +1380,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1389,24 +1401,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>